<commit_message>
add scenario 7 and 9
</commit_message>
<xml_diff>
--- a/docs/PerformanceGeneratorV2.xlsx
+++ b/docs/PerformanceGeneratorV2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaronprigal/sources/github/sample-azure-eventer/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D57116-344C-1A42-BB7D-8E4ECB1C8922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A54E82-10FD-E94E-9B98-B5AD077607A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7CFC8003-B321-4E4E-99AF-FD7AA9F6F2E9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{7CFC8003-B321-4E4E-99AF-FD7AA9F6F2E9}"/>
   </bookViews>
   <sheets>
     <sheet name="v2" sheetId="3" r:id="rId1"/>
     <sheet name="scenario 1 &amp; 3 &amp; 5" sheetId="4" r:id="rId2"/>
+    <sheet name="scenario 7 &amp; 9" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>scenario: upload  3MB file</t>
   </si>
@@ -289,10 +290,6 @@
     <t>Storage Type: general purpose v2</t>
   </si>
   <si>
-    <t>pool 1 (appender): Standard_F4s_v2 
-pool 2(generator): D4s_v3</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -659,13 +656,203 @@
   </si>
   <si>
     <t>09min28sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pool 1 (appender): Standard_F4s_v2 
+pool 2(generator): Standard_F4s_v2 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1000 files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">per sec 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>for 1 hour</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> (appender service run </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>~1 pods per node - 32 nodes f4s_v2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>eventub  1TU - 32 partitions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2000 files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">per sec 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>for 1 hour</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> (appender service run </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>~1 pods per node - 32 nodes f4s_v2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>eventub  1TU - 32 partitions</t>
+    </r>
+  </si>
+  <si>
+    <t>row 1 - scenario 7</t>
+  </si>
+  <si>
+    <t>scemario 7</t>
+  </si>
+  <si>
+    <t>scenario 9</t>
+  </si>
+  <si>
+    <t>row 2 - scenario 9</t>
+  </si>
+  <si>
+    <t>write per 1min</t>
+  </si>
+  <si>
+    <t>~59600</t>
+  </si>
+  <si>
+    <t>~1000</t>
+  </si>
+  <si>
+    <t>read per 1min</t>
+  </si>
+  <si>
+    <t>~9900</t>
+  </si>
+  <si>
+    <t>writes per sec</t>
+  </si>
+  <si>
+    <t>reads per sec</t>
+  </si>
+  <si>
+    <t>~1397</t>
+  </si>
+  <si>
+    <t>~107</t>
+  </si>
+  <si>
+    <t>calc based on 1hr granularity value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -750,8 +937,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -767,6 +962,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -799,7 +1000,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -835,6 +1036,14 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1117,6 +1326,99 @@
         <a:xfrm>
           <a:off x="0" y="7073605"/>
           <a:ext cx="15087600" cy="6553200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>377348</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FA1A5C6-24C2-F221-9BD2-69C72255F800}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="18563748" cy="7556500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{378AC9A8-12B3-4270-23E5-074FCA699D3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9398000"/>
+          <a:ext cx="14706600" cy="7480300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1425,10 +1727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF0060E-F532-F846-B1C3-67FC916E9829}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="E1" zoomScale="126" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1446,9 +1748,10 @@
     <col min="13" max="14" width="14.83203125" customWidth="1"/>
     <col min="15" max="15" width="7" customWidth="1"/>
     <col min="16" max="16" width="21" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="G1" s="13" t="s">
         <v>7</v>
       </c>
@@ -1459,12 +1762,18 @@
         <v>6</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="119" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
@@ -1479,24 +1788,30 @@
         <v>2</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="8" t="s">
         <v>8</v>
@@ -1506,7 +1821,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -1516,11 +1831,12 @@
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N3" s="9"/>
+      <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:14" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="10" t="s">
         <v>1</v>
@@ -1530,7 +1846,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -1540,15 +1856,16 @@
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N4" s="9"/>
+      <c r="P4" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J1" location="'scenario 3'!A1" display="scenario 3" xr:uid="{CAA65894-94A1-2C4E-A786-771E900710BB}"/>
-    <hyperlink ref="G1" location="'scenario 3'!A1" display="scenario 3" xr:uid="{0FDF35F5-AA23-6D4E-994B-8900EF84DD1D}"/>
-    <hyperlink ref="M1" location="'scenario 3'!A1" display="scenario 3" xr:uid="{3DED8881-A16C-904D-853C-BC789941AC40}"/>
+    <hyperlink ref="M1" location="'scenario 1 &amp; 3 &amp; 5'!A1" display="scenario 5" xr:uid="{8039042E-166E-2944-A11A-B3BE0DFE980D}"/>
+    <hyperlink ref="J1" location="'scenario 1 &amp; 3 &amp; 5'!A1" display="scenario 3" xr:uid="{313A3914-2A1B-EA48-B72B-53B5315CA1B3}"/>
+    <hyperlink ref="G1" location="'scenario 1 &amp; 3 &amp; 5'!A1" display="scenario 1" xr:uid="{118E98CB-D4FE-B24D-8611-82EF641D9935}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1560,13 +1877,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A3BF52-2960-904C-A662-3A92B7AA0CFA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
-    </sheetView>
+    <sheetView zoomScale="86" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33D65A8-6530-154B-BC81-D31F77D86AB0}">
+  <dimension ref="A39:E44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="39" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="17">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+      <c r="A41" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C42" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>